<commit_message>
categories description updates (#61)
</commit_message>
<xml_diff>
--- a/config/categories/GW portal list of icons new structure 20170317.xlsx
+++ b/config/categories/GW portal list of icons new structure 20170317.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3060" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Alt. Level 2" sheetId="1" r:id="rId1"/>
-    <sheet name="science domain categories" sheetId="2" r:id="rId2"/>
+    <sheet name="science domain categories" sheetId="2" r:id="rId1"/>
+    <sheet name="Alt. Level 2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="292">
   <si>
     <t>A - Understanding</t>
   </si>
@@ -441,9 +441,6 @@
     <t>managing</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>keyword_content</t>
   </si>
   <si>
@@ -841,6 +838,69 @@
   </si>
   <si>
     <t>4.2_evaporation_square_small.png</t>
+  </si>
+  <si>
+    <t>Where is groundwater in New Zealand? How much is there? What is its quality? How old is it?</t>
+  </si>
+  <si>
+    <t>Scientific and engineering methods that map aquifers and measure aquifer properties</t>
+  </si>
+  <si>
+    <t>What is the age of groundwater in New Zealand? Why is it measured? How is it measured?</t>
+  </si>
+  <si>
+    <t>Where do we use groundwater and how much do we use? How does land use impact groundwater? How do we manage groundwater?</t>
+  </si>
+  <si>
+    <t>Maps with locations and quantity of groundwater in New Zealand</t>
+  </si>
+  <si>
+    <t>description, with general note about type of information (maps, publications, models, etc)</t>
+  </si>
+  <si>
+    <t>Groundwater in New Zealand - the big picture: Where is it? How much is there? What is its quality? How old is it?</t>
+  </si>
+  <si>
+    <t>Notes PW</t>
+  </si>
+  <si>
+    <t>5 and 1.3</t>
+  </si>
+  <si>
+    <t>The titles are exactly the same - is the content the same?</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8</t>
+  </si>
+  <si>
+    <t>I have used questions in col E, also I've tried to indicate, broadly, the type of information that a user can find</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 and 1.2 </t>
+  </si>
+  <si>
+    <t>Titles are very similar - is the content very similar?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 </t>
+  </si>
+  <si>
+    <t>needs a better title, given 4.1 to 4.6</t>
+  </si>
+  <si>
+    <t>What methods are used to understand groundwater and its properties?</t>
+  </si>
+  <si>
+    <t>4.2 to 4.6</t>
+  </si>
+  <si>
+    <t>These duplicate 6.3 to 6.8 - do you mean this? I have set 4E the same as 6E - do you mean this?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do we protect groundwater that is used for drinking? </t>
+  </si>
+  <si>
+    <t>How do we protect ecosystems that rely on groundwater flow?</t>
   </si>
 </sst>
 </file>
@@ -887,7 +947,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -906,6 +966,60 @@
         <bgColor rgb="FFA6A6A6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -920,7 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -942,6 +1056,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1325,6 +1458,1864 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="117.140625" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="9" max="10" width="25" customWidth="1"/>
+    <col min="11" max="1025" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="H2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="H4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="H7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="E10" s="18"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" ht="30">
+      <c r="A12" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="H12" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="H14" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="H15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="E16" s="18"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="H18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="H19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30">
+      <c r="A21" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" t="s">
+        <v>167</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="H22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" t="s">
+        <v>169</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="H23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F24" t="s">
+        <v>171</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="H24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="H25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="H26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" t="s">
+        <v>177</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="H27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F28" t="s">
+        <v>179</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="H28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29" t="s">
+        <v>181</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="H30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H31" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="E32" s="18"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="18"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="10">
+        <v>3.1</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="H34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="10">
+        <v>3.2</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" t="s">
+        <v>188</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="H35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="H37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="E38" s="18"/>
+      <c r="G38" s="12"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="H40" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30">
+      <c r="A41" s="10">
+        <v>4.2</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="F41" t="s">
+        <v>190</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="H41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="10">
+        <v>4.3</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="F42" t="s">
+        <v>191</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="H42" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="H43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="F44" t="s">
+        <v>192</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="H44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="E46" s="18"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" s="18"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="10">
+        <v>5.2</v>
+      </c>
+      <c r="B49" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="F49" t="s">
+        <v>195</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="10">
+        <v>5.3</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>48</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="H50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="10">
+        <v>5.4</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="F51" t="s">
+        <v>196</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="H51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" t="s">
+        <v>50</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="H52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="10">
+        <v>5.6</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53" t="s">
+        <v>52</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="H53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="10">
+        <v>5.7</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" t="s">
+        <v>53</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="H54" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="10">
+        <v>5.8</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F55" t="s">
+        <v>197</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="H55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="10">
+        <v>5.9</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56" t="s">
+        <v>57</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="H56" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="H57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="E58" s="18"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E59" s="18"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="10">
+        <v>6.1</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F60" t="s">
+        <v>61</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="H60" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="F61" t="s">
+        <v>201</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="H61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="30">
+      <c r="A62" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="F62" t="s">
+        <v>203</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="H62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B63" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" t="s">
+        <v>73</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="H63" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" t="s">
+        <v>74</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="H64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65" t="s">
+        <v>76</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="H65" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" t="s">
+        <v>77</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B67" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="F67" t="s">
+        <v>209</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="E68" s="18"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E69" s="18"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="B70" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G70" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="H70" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B71" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" t="s">
+        <v>49</v>
+      </c>
+      <c r="G71" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="H71" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="F72" t="s">
+        <v>213</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="H72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="30">
+      <c r="A73" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="H73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B74" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="F74" t="s">
+        <v>216</v>
+      </c>
+      <c r="G74" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="H74" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B75" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="F75" t="s">
+        <v>218</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="H75" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F76" t="s">
+        <v>34</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H76" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="E77" s="18"/>
+      <c r="G77" s="12"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E78" s="18"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="10">
+        <v>8.1</v>
+      </c>
+      <c r="B79" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F79" t="s">
+        <v>82</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="H79" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B80" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="F80" t="s">
+        <v>222</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="H80" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="30">
+      <c r="A81" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B81" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H81" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="45">
+      <c r="A82" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B82" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="F82" t="s">
+        <v>226</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="H82" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B83" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F83" t="s">
+        <v>94</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="H83" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="31"/>
+      <c r="B91" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -3233,1767 +5224,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I83"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="10" width="25" customWidth="1"/>
-    <col min="11" max="1025" width="9.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="10">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="H2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="H3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30">
-      <c r="A4" s="10">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="H4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="H6" t="s">
-        <v>145</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="H7" t="s">
-        <v>145</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="H8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="H9" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" ht="30">
-      <c r="A12" s="10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="B12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="H12" t="s">
-        <v>145</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H13" t="s">
-        <v>145</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="H14" t="s">
-        <v>145</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="H15" t="s">
-        <v>145</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="10">
-        <v>2.1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>162</v>
-      </c>
-      <c r="F18" t="s">
-        <v>162</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="H18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="B19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="H19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="H20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30">
-      <c r="A21" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="B21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="H21" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>168</v>
-      </c>
-      <c r="F22" t="s">
-        <v>168</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H22" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" t="s">
-        <v>170</v>
-      </c>
-      <c r="F23" t="s">
-        <v>170</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B24" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>172</v>
-      </c>
-      <c r="F24" t="s">
-        <v>172</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>265</v>
-      </c>
-      <c r="H24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>174</v>
-      </c>
-      <c r="F25" t="s">
-        <v>174</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="H25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B26" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" t="s">
-        <v>176</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="H26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B27" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>178</v>
-      </c>
-      <c r="F27" t="s">
-        <v>178</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="H27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>180</v>
-      </c>
-      <c r="F28" t="s">
-        <v>180</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H28" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B29" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
-        <v>182</v>
-      </c>
-      <c r="F29" t="s">
-        <v>182</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="H29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" t="s">
-        <v>184</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="H30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B31" t="s">
-        <v>133</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>133</v>
-      </c>
-      <c r="F31" t="s">
-        <v>133</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="H31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="G32" s="12"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="10">
-        <v>3.1</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>188</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="H34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="10">
-        <v>3.2</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>189</v>
-      </c>
-      <c r="F35" t="s">
-        <v>189</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H36" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="10">
-        <v>3.4</v>
-      </c>
-      <c r="B37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="H37" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="G38" s="12"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="10">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="H40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="30">
-      <c r="A41" s="10">
-        <v>4.2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="F41" t="s">
-        <v>191</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="H41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="10">
-        <v>4.3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>192</v>
-      </c>
-      <c r="F42" t="s">
-        <v>192</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="H42" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="10">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B43" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="H43" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="10">
-        <v>4.5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="F44" t="s">
-        <v>193</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="H44" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="10">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B45" t="s">
-        <v>38</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="H45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="10">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B48" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" t="s">
-        <v>44</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="H48" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="10">
-        <v>5.2</v>
-      </c>
-      <c r="B49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" t="s">
-        <v>196</v>
-      </c>
-      <c r="F49" t="s">
-        <v>196</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="H49" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="10">
-        <v>5.3</v>
-      </c>
-      <c r="B50" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F50" t="s">
-        <v>48</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="H50" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="10">
-        <v>5.4</v>
-      </c>
-      <c r="B51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" t="s">
-        <v>197</v>
-      </c>
-      <c r="F51" t="s">
-        <v>197</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H51" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="10">
-        <v>5.5</v>
-      </c>
-      <c r="B52" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" t="s">
-        <v>50</v>
-      </c>
-      <c r="F52" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="H52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="10">
-        <v>5.6</v>
-      </c>
-      <c r="B53" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" t="s">
-        <v>52</v>
-      </c>
-      <c r="F53" t="s">
-        <v>52</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="H53" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="10">
-        <v>5.7</v>
-      </c>
-      <c r="B54" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" t="s">
-        <v>53</v>
-      </c>
-      <c r="F54" t="s">
-        <v>53</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="H54" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="10">
-        <v>5.8</v>
-      </c>
-      <c r="B55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" t="s">
-        <v>198</v>
-      </c>
-      <c r="F55" t="s">
-        <v>198</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="H55" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="10">
-        <v>5.9</v>
-      </c>
-      <c r="B56" t="s">
-        <v>57</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" t="s">
-        <v>57</v>
-      </c>
-      <c r="F56" t="s">
-        <v>57</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="H56" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B57" t="s">
-        <v>58</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" t="s">
-        <v>15</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="H57" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="10">
-        <v>6.1</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" t="s">
-        <v>61</v>
-      </c>
-      <c r="F60" t="s">
-        <v>61</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="H60" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C61" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="F61" t="s">
-        <v>202</v>
-      </c>
-      <c r="G61" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="H61" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="30">
-      <c r="A62" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F62" t="s">
-        <v>204</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="H62" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" t="s">
-        <v>73</v>
-      </c>
-      <c r="F63" t="s">
-        <v>73</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="H63" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F64" t="s">
-        <v>74</v>
-      </c>
-      <c r="G64" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="H64" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="B65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" t="s">
-        <v>76</v>
-      </c>
-      <c r="F65" t="s">
-        <v>76</v>
-      </c>
-      <c r="G65" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="H65" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B66" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" t="s">
-        <v>77</v>
-      </c>
-      <c r="F66" t="s">
-        <v>77</v>
-      </c>
-      <c r="G66" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="H66" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="F67" t="s">
-        <v>210</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="H67" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="10">
-        <v>7.1</v>
-      </c>
-      <c r="B70" t="s">
-        <v>45</v>
-      </c>
-      <c r="D70" t="s">
-        <v>6</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="F70" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="H70" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B71" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" t="s">
-        <v>6</v>
-      </c>
-      <c r="E71" t="s">
-        <v>49</v>
-      </c>
-      <c r="F71" t="s">
-        <v>49</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H71" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="B72" t="s">
-        <v>51</v>
-      </c>
-      <c r="D72" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" t="s">
-        <v>214</v>
-      </c>
-      <c r="F72" t="s">
-        <v>214</v>
-      </c>
-      <c r="G72" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H72" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="30">
-      <c r="A73" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" t="s">
-        <v>26</v>
-      </c>
-      <c r="F73" t="s">
-        <v>26</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="H73" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D74" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="F74" t="s">
-        <v>217</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="H74" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D75" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="F75" t="s">
-        <v>219</v>
-      </c>
-      <c r="G75" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="H75" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="B76" t="s">
-        <v>34</v>
-      </c>
-      <c r="D76" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" t="s">
-        <v>34</v>
-      </c>
-      <c r="F76" t="s">
-        <v>34</v>
-      </c>
-      <c r="G76" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="H76" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="G77" s="12"/>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="10">
-        <v>8.1</v>
-      </c>
-      <c r="B79" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" t="s">
-        <v>5</v>
-      </c>
-      <c r="D79" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" t="s">
-        <v>82</v>
-      </c>
-      <c r="F79" t="s">
-        <v>82</v>
-      </c>
-      <c r="G79" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="H79" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B80" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" t="s">
-        <v>6</v>
-      </c>
-      <c r="E80" t="s">
-        <v>223</v>
-      </c>
-      <c r="F80" t="s">
-        <v>223</v>
-      </c>
-      <c r="G80" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H80" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="30">
-      <c r="A81" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B81" t="s">
-        <v>86</v>
-      </c>
-      <c r="C81" t="s">
-        <v>5</v>
-      </c>
-      <c r="D81" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="F81" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="G81" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="H81" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="45">
-      <c r="A82" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="B82" t="s">
-        <v>23</v>
-      </c>
-      <c r="C82" t="s">
-        <v>5</v>
-      </c>
-      <c r="D82" t="s">
-        <v>6</v>
-      </c>
-      <c r="E82" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="F82" t="s">
-        <v>227</v>
-      </c>
-      <c r="G82" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="H82" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B83" t="s">
-        <v>94</v>
-      </c>
-      <c r="C83" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" t="s">
-        <v>6</v>
-      </c>
-      <c r="E83" t="s">
-        <v>94</v>
-      </c>
-      <c r="F83" t="s">
-        <v>94</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="H83" t="s">
-        <v>145</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>